<commit_message>
Docs: API 설계서 update
</commit_message>
<xml_diff>
--- a/api 설계서.xlsx
+++ b/api 설계서.xlsx
@@ -5,14 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSAFY\workspace\08_Framework\관통\enjoytrip_09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSAFY\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8925"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1 (3)" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1 (4)" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
   <si>
     <t>게시판</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,43 +112,222 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>마이페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탈퇴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board/articleNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board/{key}/{word}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board/regist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/user/info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"title":"", "content":"", "file":file}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/user/regist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"id":"", "pwd":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"id":"", "pwd":"", "name":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 일반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"content_type_id":0, "title":"", "addr1":"", "first_image":"", "latitude":BigDecimal, "longitude":BigDecimal}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여행지 검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구군 코드 검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/trip/{sido}/{gugun}/{contentType}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/trip/{sido}</t>
+  </si>
+  <si>
+    <t>/user/login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/user/delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>계획</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>GET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북마크 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북마크 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/plan/{planId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/plan/{planId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/plan/regist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/plan/{word}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/user/mark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>GET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>/user/update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"title":"", "content":"", "file":file}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"title":"", "plan_list":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"title":"", "plan_list":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"title":"", "plan_list":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인정보 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"id":"", "pwd":"", "name":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북마크 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/user/mark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북마크 상세정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>GET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>마이페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탈퇴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DELETE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/board</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/board/articleNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/board/{key}/{word}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파일 다운로드</t>
+    <t>/user/mark/{planId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/user/mark/{planId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세보기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -153,78 +335,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/board/regist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/user/info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"title":"", "content":"", "file":file}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/user/regist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"id":"", "pwd":""}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"id":"", "pwd":"", "name":""}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>- 일반</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/board/{sfolder}/{ofile}/{sfile}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"content_type_id":0, "title":"", "addr1":"", "first_image":"", "latitude":BigDecimal, "longitude":BigDecimal}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>여행지 검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구군 코드 검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/trip/{sido}/{gugun}/{contentType}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/trip/{sido}</t>
-  </si>
-  <si>
-    <t>/user/login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/user/update</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/user/delete</t>
+    <t>/plan/{planId}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -232,7 +343,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +356,22 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -280,7 +407,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -291,6 +418,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -573,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G35"/>
+  <dimension ref="B4:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -619,24 +752,24 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>35</v>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -647,7 +780,7 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -658,182 +791,426 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="15.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="62.625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="15.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="62.625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="15.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="62.625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>